<commit_message>
update 3.6 data pemberdayaan, update data anggota cu
</commit_message>
<xml_diff>
--- a/public/files/formatProdukAnggotaCu.xlsx
+++ b/public/files/formatProdukAnggotaCu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411E82E7-D97A-814B-AA9E-5C708C304A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76A5FB2-6EC9-474F-AC34-06776BF49B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1460" windowWidth="27640" windowHeight="16540" xr2:uid="{29C24AB3-ADF9-6E47-9BED-236D5A200869}"/>
   </bookViews>
@@ -39,7 +39,6 @@
     <author>tc={772FA2DA-AD02-D649-95EE-AEB9E17CCEF1}</author>
     <author>tc={6D341D79-53BD-EE44-97E0-3FD031E66640}</author>
     <author>tc={4A4B588A-5FA4-904E-BC55-BBCEC379F516}</author>
-    <author>tc={42BB0132-5A04-5446-942E-1906A54AEFFE}</author>
     <author>tc={FF90BD73-3505-004C-A2E2-2A75E23EB93E}</author>
     <author>tc={148B8BDA-78E0-8042-A8A6-8D585C2B6A85}</author>
     <author>tc={616E2D4C-C225-7549-914B-10076EA9B79A}</author>
@@ -80,15 +79,7 @@
     kode produk harus sesuai dengan yang ada di produk cu di SIMO</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{42BB0132-5A04-5446-942E-1906A54AEFFE}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    saldo akhir</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{FF90BD73-3505-004C-A2E2-2A75E23EB93E}">
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{FF90BD73-3505-004C-A2E2-2A75E23EB93E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +88,7 @@
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{148B8BDA-78E0-8042-A8A6-8D585C2B6A85}">
+    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{148B8BDA-78E0-8042-A8A6-8D585C2B6A85}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +96,7 @@
     tanggal transaksi sesuai perubahan saldo</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{616E2D4C-C225-7549-914B-10076EA9B79A}">
+    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{616E2D4C-C225-7549-914B-10076EA9B79A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +105,7 @@
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{EAF9B473-D23D-C541-BAE9-C5304A07C7EA}">
+    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{EAF9B473-D23D-C541-BAE9-C5304A07C7EA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -122,7 +113,7 @@
     berapa lama lagi pinjaman ini akan selesai? diisi dengan angka dalam satuan bulan</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{6BB14561-B21B-944D-908F-84C2D4523712}">
+    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{6BB14561-B21B-944D-908F-84C2D4523712}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +122,7 @@
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{574137E0-CC07-D54B-A72B-04A03F3B737D}">
+    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{574137E0-CC07-D54B-A72B-04A03F3B737D}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>no_ba</t>
   </si>
@@ -160,9 +151,6 @@
     <t>kode_produk</t>
   </si>
   <si>
-    <t>saldo</t>
-  </si>
-  <si>
     <t>tanggal_transaksi</t>
   </si>
   <si>
@@ -179,6 +167,12 @@
   </si>
   <si>
     <t>tanggal_buka</t>
+  </si>
+  <si>
+    <t>dpd</t>
+  </si>
+  <si>
+    <t>kolekbi</t>
   </si>
 </sst>
 </file>
@@ -236,7 +230,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,9 +255,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,7 +295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -407,7 +401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -549,7 +543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,28 +563,25 @@
   <threadedComment ref="D1" dT="2020-09-21T03:33:22.63" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{4A4B588A-5FA4-904E-BC55-BBCEC379F516}">
     <text>kode produk harus sesuai dengan yang ada di produk cu di SIMO</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2020-09-21T03:39:48.67" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{42BB0132-5A04-5446-942E-1906A54AEFFE}">
-    <text>saldo akhir</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2020-09-21T03:35:02.04" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{FF90BD73-3505-004C-A2E2-2A75E23EB93E}">
+  <threadedComment ref="E1" dT="2020-09-21T03:35:02.04" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{FF90BD73-3505-004C-A2E2-2A75E23EB93E}">
     <text>tanggal buka rekening
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</text>
   </threadedComment>
-  <threadedComment ref="G1" dT="2020-09-21T03:35:59.37" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{148B8BDA-78E0-8042-A8A6-8D585C2B6A85}">
+  <threadedComment ref="F1" dT="2020-09-21T03:35:59.37" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{148B8BDA-78E0-8042-A8A6-8D585C2B6A85}">
     <text>tanggal transaksi sesuai perubahan saldo</text>
   </threadedComment>
-  <threadedComment ref="H1" dT="2020-09-21T03:36:35.56" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{616E2D4C-C225-7549-914B-10076EA9B79A}">
+  <threadedComment ref="G1" dT="2020-09-21T03:36:35.56" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{616E2D4C-C225-7549-914B-10076EA9B79A}">
     <text>lama pinjaman sesuai perjanjian, diisi dengan angka dalam satuan bulan
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2020-09-21T03:37:24.75" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{EAF9B473-D23D-C541-BAE9-C5304A07C7EA}">
+  <threadedComment ref="H1" dT="2020-09-21T03:37:24.75" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{EAF9B473-D23D-C541-BAE9-C5304A07C7EA}">
     <text>berapa lama lagi pinjaman ini akan selesai? diisi dengan angka dalam satuan bulan</text>
   </threadedComment>
-  <threadedComment ref="J1" dT="2020-09-21T03:39:31.22" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{6BB14561-B21B-944D-908F-84C2D4523712}">
+  <threadedComment ref="I1" dT="2020-09-21T03:39:31.22" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{6BB14561-B21B-944D-908F-84C2D4523712}">
     <text>tujuan pembukaan rekening ini
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO</text>
   </threadedComment>
-  <threadedComment ref="K1" dT="2020-09-21T03:39:15.33" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{574137E0-CC07-D54B-A72B-04A03F3B737D}">
+  <threadedComment ref="J1" dT="2020-09-21T03:39:15.33" personId="{54F23C19-E5B6-1C47-9F11-B1D2B540C282}" id="{574137E0-CC07-D54B-A72B-04A03F3B737D}">
     <text xml:space="preserve">Untuk simpanan rencana khusus (mis: kendaraan, perumahan) dan diisi dengan tanggal kapan rencana tersebut akan tercapai
 boleh dikosongkan jika rekening ini sudah ada sebelumnya di SIMO
 </text>
@@ -600,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEAE8A1-4B4A-5848-8FCE-5E0FF7B94A5A}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,16 +602,15 @@
     <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="2"/>
-    <col min="11" max="11" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,26 +623,29 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>